<commit_message>
13.04.19 Today 10:33 PM Last Updated
</commit_message>
<xml_diff>
--- a/Symphony Update Price List 11.4.19.xlsx
+++ b/Symphony Update Price List 11.4.19.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="93">
   <si>
     <t>B12i</t>
   </si>
@@ -289,7 +289,10 @@
     <t>100 lifting marging &amp; 30 Back Margin</t>
   </si>
   <si>
-    <t>Symphony Update Price list                              Date: 11.4.19</t>
+    <t>Symphony Update Price list                              Date: 13.4.19</t>
+  </si>
+  <si>
+    <t>Package 5 Offer</t>
   </si>
 </sst>
 </file>
@@ -299,7 +302,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -365,6 +368,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -381,7 +397,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.34998626667073579"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -428,7 +444,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -480,6 +496,12 @@
     </xf>
     <xf numFmtId="3" fontId="5" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -785,26 +807,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22" defaultRowHeight="18.75"/>
   <cols>
     <col min="1" max="1" width="8.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="7.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23" style="4" customWidth="1"/>
-    <col min="5" max="5" width="5.140625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="22" style="4"/>
+    <col min="4" max="4" width="9.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="5.140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24" style="4" customWidth="1"/>
+    <col min="11" max="16384" width="22" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30.75" customHeight="1">
+    <row r="1" spans="1:10" ht="30.75" customHeight="1">
       <c r="A1" s="12" t="s">
         <v>91</v>
       </c>
@@ -816,8 +839,9 @@
       <c r="G1" s="12"/>
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
-    </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" ht="37.5">
+      <c r="J1" s="12"/>
+    </row>
+    <row r="2" spans="1:10" s="2" customFormat="1" ht="37.5">
       <c r="A2" s="1" t="s">
         <v>44</v>
       </c>
@@ -827,23 +851,26 @@
       <c r="C2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -853,21 +880,22 @@
       <c r="C3" s="3">
         <v>875</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="3"/>
+      <c r="E3" s="3">
         <v>10</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="G3" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="G3" s="8">
+      <c r="H3" s="8">
         <v>1730</v>
       </c>
-      <c r="H3" s="8">
+      <c r="I3" s="8">
         <v>1890</v>
       </c>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="3" t="s">
         <v>75</v>
       </c>
@@ -878,20 +906,21 @@
         <v>925</v>
       </c>
       <c r="D4" s="3"/>
-      <c r="F4" s="3" t="s">
+      <c r="E4" s="3"/>
+      <c r="G4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="5">
+      <c r="H4" s="5">
         <v>1250</v>
       </c>
-      <c r="H4" s="5">
+      <c r="I4" s="5">
         <v>1350</v>
       </c>
-      <c r="I4" s="3">
+      <c r="J4" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" s="3" t="s">
         <v>68</v>
       </c>
@@ -901,23 +930,25 @@
       <c r="C5" s="3">
         <v>880</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="3"/>
+      <c r="E5" s="3">
         <v>10</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="18"/>
+      <c r="G5" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G5" s="5">
+      <c r="H5" s="5">
         <v>1370</v>
       </c>
-      <c r="H5" s="5">
+      <c r="I5" s="5">
         <v>1490</v>
       </c>
-      <c r="I5" s="3">
+      <c r="J5" s="3">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
@@ -927,23 +958,24 @@
       <c r="C6" s="3">
         <v>870</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3">
         <v>10</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="5">
+      <c r="H6" s="5">
         <v>1890</v>
       </c>
-      <c r="H6" s="5">
+      <c r="I6" s="5">
         <v>2090</v>
       </c>
-      <c r="I6" s="3">
+      <c r="J6" s="3">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="37.5">
+    <row r="7" spans="1:10" ht="37.5">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -953,47 +985,51 @@
       <c r="C7" s="3">
         <v>865</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="3"/>
+      <c r="E7" s="3">
         <v>10</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="G7" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="14">
+      <c r="H7" s="14">
         <v>2780</v>
       </c>
-      <c r="H7" s="15">
+      <c r="I7" s="15">
         <v>2990</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="J7" s="13" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:10">
+      <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="13">
         <v>790</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="13">
         <v>860</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="13">
+        <v>30</v>
+      </c>
+      <c r="E8" s="13">
         <v>10</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="G8" s="5">
+      <c r="H8" s="5">
         <v>6540</v>
       </c>
-      <c r="H8" s="5">
+      <c r="I8" s="5">
         <v>6990</v>
       </c>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="3" t="s">
         <v>77</v>
       </c>
@@ -1004,20 +1040,21 @@
         <v>990</v>
       </c>
       <c r="D9" s="3"/>
-      <c r="F9" s="3" t="s">
+      <c r="E9" s="3"/>
+      <c r="G9" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G9" s="5">
+      <c r="H9" s="5">
         <v>6210</v>
       </c>
-      <c r="H9" s="5">
+      <c r="I9" s="5">
         <v>6690</v>
       </c>
-      <c r="I9" s="3">
+      <c r="J9" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10">
       <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
@@ -1027,23 +1064,24 @@
       <c r="C10" s="3">
         <v>980</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="3"/>
+      <c r="E10" s="3">
         <v>10</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="G10" s="5">
+      <c r="H10" s="5">
         <v>7075</v>
       </c>
-      <c r="H10" s="5">
+      <c r="I10" s="5">
         <v>7575</v>
       </c>
-      <c r="I10" s="3">
+      <c r="J10" s="3">
         <v>145</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10">
       <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
@@ -1053,23 +1091,24 @@
       <c r="C11" s="3">
         <v>970</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="3"/>
+      <c r="E11" s="3">
         <v>10</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="G11" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G11" s="5">
+      <c r="H11" s="5">
         <v>7910</v>
       </c>
-      <c r="H11" s="5">
+      <c r="I11" s="5">
         <v>8490</v>
       </c>
-      <c r="I11" s="3">
+      <c r="J11" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:10">
       <c r="A12" s="3" t="s">
         <v>80</v>
       </c>
@@ -1080,46 +1119,50 @@
         <v>999</v>
       </c>
       <c r="D12" s="3"/>
-      <c r="F12" s="13" t="s">
+      <c r="E12" s="3"/>
+      <c r="G12" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="G12" s="16">
+      <c r="H12" s="16">
         <v>7890</v>
       </c>
-      <c r="H12" s="16">
+      <c r="I12" s="16">
         <v>8490</v>
       </c>
-      <c r="I12" s="13" t="s">
+      <c r="J12" s="13" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:10">
+      <c r="A13" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="13">
         <v>880</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="13">
         <v>950</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="13">
+        <v>40</v>
+      </c>
+      <c r="E13" s="13">
         <v>20</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="G13" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="G13" s="16">
+      <c r="H13" s="16">
         <v>7490</v>
       </c>
-      <c r="H13" s="16">
+      <c r="I13" s="16">
         <v>7990</v>
       </c>
-      <c r="I13" s="13" t="s">
+      <c r="J13" s="13" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:10">
       <c r="A14" s="3" t="s">
         <v>8</v>
       </c>
@@ -1129,23 +1172,24 @@
       <c r="C14" s="5">
         <v>1095</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="5"/>
+      <c r="E14" s="3">
         <v>25</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="G14" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="G14" s="5">
+      <c r="H14" s="5">
         <v>8340</v>
       </c>
-      <c r="H14" s="5">
+      <c r="I14" s="5">
         <v>8990</v>
       </c>
-      <c r="I14" s="3">
+      <c r="J14" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:10">
       <c r="A15" s="3" t="s">
         <v>10</v>
       </c>
@@ -1155,23 +1199,24 @@
       <c r="C15" s="3">
         <v>1060</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="3"/>
+      <c r="E15" s="3">
         <v>10</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="G15" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G15" s="5">
+      <c r="H15" s="5">
         <v>9190</v>
       </c>
-      <c r="H15" s="5">
+      <c r="I15" s="5">
         <v>9990</v>
       </c>
-      <c r="I15" s="3">
+      <c r="J15" s="3">
         <v>170</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:10">
       <c r="A16" s="3" t="s">
         <v>76</v>
       </c>
@@ -1182,20 +1227,21 @@
         <v>1090</v>
       </c>
       <c r="D16" s="3"/>
-      <c r="F16" s="3" t="s">
+      <c r="E16" s="3"/>
+      <c r="G16" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G16" s="5">
+      <c r="H16" s="5">
         <v>3560</v>
       </c>
-      <c r="H16" s="5">
+      <c r="I16" s="5">
         <v>3840</v>
       </c>
-      <c r="I16" s="3">
+      <c r="J16" s="3">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="37.5">
+    <row r="17" spans="1:10" ht="37.5">
       <c r="A17" s="3" t="s">
         <v>79</v>
       </c>
@@ -1206,20 +1252,21 @@
         <v>1075</v>
       </c>
       <c r="D17" s="3"/>
-      <c r="F17" s="13" t="s">
+      <c r="E17" s="3"/>
+      <c r="G17" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="G17" s="16">
+      <c r="H17" s="16">
         <v>3340</v>
       </c>
-      <c r="H17" s="16">
+      <c r="I17" s="16">
         <v>3590</v>
       </c>
-      <c r="I17" s="13" t="s">
+      <c r="J17" s="13" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:10">
       <c r="A18" s="3" t="s">
         <v>19</v>
       </c>
@@ -1229,23 +1276,24 @@
       <c r="C18" s="5">
         <v>1090</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="5"/>
+      <c r="E18" s="3">
         <v>10</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="G18" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G18" s="5">
+      <c r="H18" s="5">
         <v>4690</v>
       </c>
-      <c r="H18" s="5">
+      <c r="I18" s="5">
         <v>4999</v>
       </c>
-      <c r="I18" s="3">
+      <c r="J18" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:10">
       <c r="A19" s="3" t="s">
         <v>78</v>
       </c>
@@ -1255,23 +1303,24 @@
       <c r="C19" s="5">
         <v>1040</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="5"/>
+      <c r="E19" s="3">
         <v>10</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="G19" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G19" s="5">
+      <c r="H19" s="5">
         <v>5390</v>
       </c>
-      <c r="H19" s="5">
+      <c r="I19" s="5">
         <v>5790</v>
       </c>
-      <c r="I19" s="3">
+      <c r="J19" s="3">
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:10">
       <c r="A20" s="3" t="s">
         <v>21</v>
       </c>
@@ -1281,23 +1330,24 @@
       <c r="C20" s="3">
         <v>1070</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="3"/>
+      <c r="E20" s="3">
         <v>10</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="G20" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G20" s="5">
+      <c r="H20" s="5">
         <v>4970</v>
       </c>
-      <c r="H20" s="5">
+      <c r="I20" s="5">
         <v>5290</v>
       </c>
-      <c r="I20" s="3">
+      <c r="J20" s="3">
         <v>130</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="37.5">
+    <row r="21" spans="1:10" ht="37.5">
       <c r="A21" s="3" t="s">
         <v>74</v>
       </c>
@@ -1307,49 +1357,53 @@
       <c r="C21" s="3">
         <v>1120</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="3"/>
+      <c r="E21" s="3">
         <v>20</v>
       </c>
-      <c r="F21" s="13" t="s">
+      <c r="G21" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="G21" s="15">
+      <c r="H21" s="15">
         <v>3710</v>
       </c>
-      <c r="H21" s="17">
+      <c r="I21" s="17">
         <v>3990</v>
       </c>
-      <c r="I21" s="13" t="s">
+      <c r="J21" s="13" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="37.5">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:10" ht="37.5">
+      <c r="A22" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="16">
         <v>1290</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="16">
         <v>1390</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="16">
+        <v>100</v>
+      </c>
+      <c r="E22" s="13">
         <v>10</v>
       </c>
-      <c r="F22" s="13" t="s">
+      <c r="G22" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="G22" s="15">
+      <c r="H22" s="15">
         <v>3620</v>
       </c>
-      <c r="H22" s="17">
+      <c r="I22" s="17">
         <v>3890</v>
       </c>
-      <c r="I22" s="13" t="s">
+      <c r="J22" s="13" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:10">
       <c r="A23" s="3" t="s">
         <v>25</v>
       </c>
@@ -1359,23 +1413,24 @@
       <c r="C23" s="5">
         <v>1370</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="5"/>
+      <c r="E23" s="3">
         <v>10</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="G23" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G23" s="9">
+      <c r="H23" s="9">
         <v>4620</v>
       </c>
-      <c r="H23" s="9">
+      <c r="I23" s="9">
         <v>4999</v>
       </c>
-      <c r="I23" s="3">
+      <c r="J23" s="3">
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="20.25" customHeight="1">
+    <row r="24" spans="1:10" ht="20.25" customHeight="1">
       <c r="A24" s="3" t="s">
         <v>26</v>
       </c>
@@ -1385,23 +1440,24 @@
       <c r="C24" s="5">
         <v>1290</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="5"/>
+      <c r="E24" s="3">
         <v>10</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="G24" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G24" s="9">
+      <c r="H24" s="9">
         <v>4520</v>
       </c>
-      <c r="H24" s="9">
+      <c r="I24" s="9">
         <v>4899</v>
       </c>
-      <c r="I24" s="3">
+      <c r="J24" s="3">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="21" customHeight="1">
+    <row r="25" spans="1:10" ht="21" customHeight="1">
       <c r="A25" s="3" t="s">
         <v>48</v>
       </c>
@@ -1411,23 +1467,24 @@
       <c r="C25" s="5">
         <v>1390</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="5"/>
+      <c r="E25" s="3">
         <v>25</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="G25" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G25" s="10">
+      <c r="H25" s="10">
         <v>4080</v>
       </c>
-      <c r="H25" s="11">
+      <c r="I25" s="11">
         <v>4390</v>
       </c>
-      <c r="I25" s="3">
+      <c r="J25" s="3">
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="18.75" customHeight="1">
+    <row r="26" spans="1:10" ht="18.75" customHeight="1">
       <c r="A26" s="3" t="s">
         <v>47</v>
       </c>
@@ -1437,23 +1494,24 @@
       <c r="C26" s="5">
         <v>1290</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="5"/>
+      <c r="E26" s="3">
         <v>50</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="G26" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G26" s="9">
+      <c r="H26" s="9">
         <v>4360</v>
       </c>
-      <c r="H26" s="9">
+      <c r="I26" s="9">
         <v>4740</v>
       </c>
-      <c r="I26" s="3">
+      <c r="J26" s="3">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:10">
       <c r="A27" s="3" t="s">
         <v>1</v>
       </c>
@@ -1463,49 +1521,53 @@
       <c r="C27" s="5">
         <v>1160</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="5"/>
+      <c r="E27" s="3">
         <v>10</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="G27" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="G27" s="10">
+      <c r="H27" s="10">
         <v>4640</v>
       </c>
-      <c r="H27" s="11">
+      <c r="I27" s="11">
         <v>4990</v>
       </c>
-      <c r="I27" s="3">
+      <c r="J27" s="3">
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="3" t="s">
+    <row r="28" spans="1:10">
+      <c r="A28" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="16">
         <v>1100</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C28" s="16">
         <v>1199</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="16">
+        <v>50</v>
+      </c>
+      <c r="E28" s="13">
         <v>20</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="G28" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G28" s="5">
+      <c r="H28" s="5">
         <v>5650</v>
       </c>
-      <c r="H28" s="5">
+      <c r="I28" s="5">
         <v>6150</v>
       </c>
-      <c r="I28" s="3">
+      <c r="J28" s="3">
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:10">
       <c r="A29" s="3" t="s">
         <v>4</v>
       </c>
@@ -1515,23 +1577,24 @@
       <c r="C29" s="5">
         <v>1220</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="5"/>
+      <c r="E29" s="3">
         <v>20</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="G29" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G29" s="5">
+      <c r="H29" s="5">
         <v>5020</v>
       </c>
-      <c r="H29" s="5">
+      <c r="I29" s="5">
         <v>5390</v>
       </c>
-      <c r="I29" s="3">
+      <c r="J29" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:10">
       <c r="A30" s="3" t="s">
         <v>6</v>
       </c>
@@ -1541,23 +1604,24 @@
       <c r="C30" s="5">
         <v>1130</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30" s="5"/>
+      <c r="E30" s="3">
         <v>20</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="G30" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G30" s="5">
+      <c r="H30" s="5">
         <v>5280</v>
       </c>
-      <c r="H30" s="5">
+      <c r="I30" s="5">
         <v>5690</v>
       </c>
-      <c r="I30" s="3">
+      <c r="J30" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="37.5">
+    <row r="31" spans="1:10" ht="37.5">
       <c r="A31" s="3" t="s">
         <v>58</v>
       </c>
@@ -1567,23 +1631,24 @@
       <c r="C31" s="5">
         <v>1199</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31" s="5"/>
+      <c r="E31" s="3">
         <v>20</v>
       </c>
-      <c r="F31" s="13" t="s">
+      <c r="G31" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="G31" s="16">
+      <c r="H31" s="16">
         <v>5440</v>
       </c>
-      <c r="H31" s="16">
+      <c r="I31" s="16">
         <v>5840</v>
       </c>
-      <c r="I31" s="13" t="s">
+      <c r="J31" s="13" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="37.5">
+    <row r="32" spans="1:10" ht="37.5">
       <c r="A32" s="3" t="s">
         <v>83</v>
       </c>
@@ -1593,21 +1658,22 @@
       <c r="C32" s="5">
         <v>1199</v>
       </c>
-      <c r="D32" s="3"/>
-      <c r="F32" s="13" t="s">
+      <c r="D32" s="5"/>
+      <c r="E32" s="3"/>
+      <c r="G32" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="G32" s="16">
+      <c r="H32" s="16">
         <v>5560</v>
       </c>
-      <c r="H32" s="16">
+      <c r="I32" s="16">
         <v>5990</v>
       </c>
-      <c r="I32" s="13" t="s">
+      <c r="J32" s="13" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="18.75" customHeight="1">
+    <row r="33" spans="1:10" ht="18.75" customHeight="1">
       <c r="A33" s="3" t="s">
         <v>9</v>
       </c>
@@ -1617,49 +1683,53 @@
       <c r="C33" s="5">
         <v>1230</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D33" s="5"/>
+      <c r="E33" s="3">
         <v>10</v>
       </c>
-      <c r="F33" s="6" t="s">
+      <c r="G33" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G33" s="7">
+      <c r="H33" s="7">
         <v>6090</v>
       </c>
-      <c r="H33" s="7">
+      <c r="I33" s="7">
         <v>6590</v>
       </c>
-      <c r="I33" s="6">
+      <c r="J33" s="6">
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="3" t="s">
+    <row r="34" spans="1:10">
+      <c r="A34" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="5">
+      <c r="B34" s="16">
         <v>1100</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C34" s="16">
         <v>1190</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34" s="16">
+        <v>50</v>
+      </c>
+      <c r="E34" s="13">
         <v>10</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="G34" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G34" s="5">
+      <c r="H34" s="5">
         <v>5390</v>
       </c>
-      <c r="H34" s="5">
+      <c r="I34" s="5">
         <v>5790</v>
       </c>
-      <c r="I34" s="3">
+      <c r="J34" s="3">
         <v>120</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:10">
       <c r="A35" s="3" t="s">
         <v>50</v>
       </c>
@@ -1669,47 +1739,51 @@
       <c r="C35" s="5">
         <v>1450</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D35" s="5"/>
+      <c r="E35" s="3">
         <v>50</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="G35" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G35" s="5">
+      <c r="H35" s="5">
         <v>12590</v>
       </c>
-      <c r="H35" s="5">
+      <c r="I35" s="5">
         <v>13490</v>
       </c>
-      <c r="I35" s="3"/>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="A36" s="3" t="s">
+      <c r="J35" s="3"/>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="5">
+      <c r="B36" s="16">
         <v>1330</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C36" s="16">
         <v>1450</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D36" s="16">
+        <v>100</v>
+      </c>
+      <c r="E36" s="13">
         <v>20</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="G36" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G36" s="5">
+      <c r="H36" s="5">
         <v>12240</v>
       </c>
-      <c r="H36" s="5">
+      <c r="I36" s="5">
         <v>12990</v>
       </c>
-      <c r="I36" s="3">
+      <c r="J36" s="3">
         <v>350</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:10">
       <c r="A37" s="3" t="s">
         <v>12</v>
       </c>
@@ -1719,23 +1793,24 @@
       <c r="C37" s="5">
         <v>1299</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D37" s="5"/>
+      <c r="E37" s="3">
         <v>20</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="G37" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G37" s="5">
+      <c r="H37" s="5">
         <v>12090</v>
       </c>
-      <c r="H37" s="5">
+      <c r="I37" s="5">
         <v>12990</v>
       </c>
-      <c r="I37" s="3">
+      <c r="J37" s="3">
         <v>200</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:10">
       <c r="A38" s="3" t="s">
         <v>38</v>
       </c>
@@ -1745,23 +1820,24 @@
       <c r="C38" s="5">
         <v>1320</v>
       </c>
-      <c r="D38" s="3">
+      <c r="D38" s="5"/>
+      <c r="E38" s="3">
         <v>20</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="G38" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G38" s="5">
+      <c r="H38" s="5">
         <v>10840</v>
       </c>
-      <c r="H38" s="5">
+      <c r="I38" s="5">
         <v>11990</v>
       </c>
-      <c r="I38" s="3">
+      <c r="J38" s="3">
         <v>200</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:10">
       <c r="A39" s="3" t="s">
         <v>40</v>
       </c>
@@ -1771,23 +1847,24 @@
       <c r="C39" s="5">
         <v>1590</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D39" s="5"/>
+      <c r="E39" s="3">
         <v>20</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="G39" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G39" s="5">
+      <c r="H39" s="5">
         <v>12490</v>
       </c>
-      <c r="H39" s="5">
+      <c r="I39" s="5">
         <v>13490</v>
       </c>
-      <c r="I39" s="3">
+      <c r="J39" s="3">
         <v>300</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:10">
       <c r="A40" s="3" t="s">
         <v>42</v>
       </c>
@@ -1797,23 +1874,24 @@
       <c r="C40" s="5">
         <v>1590</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D40" s="5"/>
+      <c r="E40" s="3">
         <v>60</v>
       </c>
-      <c r="F40" s="3" t="s">
+      <c r="G40" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="G40" s="5">
+      <c r="H40" s="5">
         <v>12800</v>
       </c>
-      <c r="H40" s="5">
+      <c r="I40" s="5">
         <v>13990</v>
       </c>
-      <c r="I40" s="3">
+      <c r="J40" s="3">
         <v>250</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:10">
       <c r="A41" s="3" t="s">
         <v>51</v>
       </c>
@@ -1823,23 +1901,24 @@
       <c r="C41" s="5">
         <v>1740</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D41" s="5"/>
+      <c r="E41" s="3">
         <v>50</v>
       </c>
-      <c r="F41" s="3" t="s">
+      <c r="G41" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G41" s="5">
+      <c r="H41" s="5">
         <v>17790</v>
       </c>
-      <c r="H41" s="5">
+      <c r="I41" s="5">
         <v>18990</v>
       </c>
-      <c r="I41" s="3">
+      <c r="J41" s="3">
         <v>300</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:10">
       <c r="A42" s="3" t="s">
         <v>24</v>
       </c>
@@ -1849,19 +1928,20 @@
       <c r="C42" s="5">
         <v>1590</v>
       </c>
-      <c r="D42" s="3">
+      <c r="D42" s="5"/>
+      <c r="E42" s="3">
         <v>40</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="G42" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G42" s="5">
+      <c r="H42" s="5">
         <v>7740</v>
       </c>
-      <c r="H42" s="5">
+      <c r="I42" s="5">
         <v>8490</v>
       </c>
-      <c r="I42" s="3">
+      <c r="J42" s="3">
         <v>150</v>
       </c>
     </row>
@@ -1870,9 +1950,10 @@
     <sortCondition ref="A2:A69"/>
   </sortState>
   <mergeCells count="1">
-    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A1:J1"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions verticalCentered="1"/>
+  <pageMargins left="0.75" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>